<commit_message>
feat: AG Grid 전환 및 Claude API 화면 생성 완료
### 주요 변경사항
- RealGrid → AG Grid 전환 결정 및 구현
- Claude API 기반 화면 자동 생성 스크립트 완성
- SC002 (제품 수불 관리), SC008 (판매관리비 집계표) 화면 생성
- AG Grid 5가지 스타일 예제 추가

### 해결한 문제
- AG Grid 모듈 등록 패턴 적용
- dotenv override 옵션으로 환경 변수 문제 해결
- Enterprise 전용 옵션 제거 (enableRangeSelection)
- TypeScript 타입 및 shadcn/ui Select 호환성 수정

### 문서화
- docs/AG_GRID_DECISION.md: AG Grid 선택 근거
- docs/SESSION_SUMMARY_20251204.md: 오늘 작업 요약
- ENVIRONMENT.md: 환경 변수 문제 해결 방법 추가
</commit_message>
<xml_diff>
--- a/data/sample_excel/부서별_원가_분석.xlsx
+++ b/data/sample_excel/부서별_원가_분석.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="부서별원가분석" sheetId="1" r:id="rId1"/>
+    <sheet name="부서별원가" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,207 +397,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>년월</v>
+      </c>
+      <c r="B1" t="str">
         <v>부서코드</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>부서명</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>제품코드</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>제품명</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>원가</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>수량</v>
-      </c>
-      <c r="G1" t="str">
-        <v>작업시간</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>202411</v>
+      </c>
+      <c r="B2" t="str">
         <v>D001</v>
       </c>
-      <c r="B2" t="str">
-        <v>생산1부</v>
-      </c>
       <c r="C2" t="str">
-        <v>P001</v>
+        <v>생산1팀</v>
       </c>
       <c r="D2" t="str">
-        <v>제품A</v>
-      </c>
-      <c r="E2">
+        <v>MDL-001</v>
+      </c>
+      <c r="E2" t="str">
+        <v>디스플레이 패널</v>
+      </c>
+      <c r="F2">
         <v>15000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>100</v>
-      </c>
-      <c r="G2">
-        <v>8.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>D001</v>
+        <v>202411</v>
       </c>
       <c r="B3" t="str">
-        <v>생산1부</v>
+        <v>D002</v>
       </c>
       <c r="C3" t="str">
-        <v>P002</v>
+        <v>생산2팀</v>
       </c>
       <c r="D3" t="str">
-        <v>제품B</v>
-      </c>
-      <c r="E3">
-        <v>25000</v>
+        <v>MDL-002</v>
+      </c>
+      <c r="E3" t="str">
+        <v>LED 모듈</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>8000</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>D002</v>
+        <v>202411</v>
       </c>
       <c r="B4" t="str">
-        <v>생산2부</v>
+        <v>D003</v>
       </c>
       <c r="C4" t="str">
-        <v>P003</v>
+        <v>품질관리팀</v>
       </c>
       <c r="D4" t="str">
-        <v>제품C</v>
-      </c>
-      <c r="E4">
-        <v>30000</v>
+        <v>MDL-003</v>
+      </c>
+      <c r="E4" t="str">
+        <v>컨트롤러</v>
       </c>
       <c r="F4">
-        <v>75</v>
+        <v>12000</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>D002</v>
-      </c>
-      <c r="B5" t="str">
-        <v>생산2부</v>
-      </c>
-      <c r="C5" t="str">
-        <v>P004</v>
-      </c>
-      <c r="D5" t="str">
-        <v>제품D</v>
-      </c>
-      <c r="E5">
-        <v>18000</v>
-      </c>
-      <c r="F5">
-        <v>120</v>
-      </c>
-      <c r="G5">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>D003</v>
-      </c>
-      <c r="B6" t="str">
-        <v>품질관리부</v>
-      </c>
-      <c r="C6" t="str">
-        <v>P001</v>
-      </c>
-      <c r="D6" t="str">
-        <v>제품A</v>
-      </c>
-      <c r="E6">
-        <v>5000</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>D003</v>
-      </c>
-      <c r="B7" t="str">
-        <v>품질관리부</v>
-      </c>
-      <c r="C7" t="str">
-        <v>P002</v>
-      </c>
-      <c r="D7" t="str">
-        <v>제품B</v>
-      </c>
-      <c r="E7">
-        <v>5000</v>
-      </c>
-      <c r="F7">
-        <v>50</v>
-      </c>
-      <c r="G7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>D004</v>
-      </c>
-      <c r="B8" t="str">
-        <v>자재관리부</v>
-      </c>
-      <c r="C8" t="str">
-        <v>P005</v>
-      </c>
-      <c r="D8" t="str">
-        <v>제품E</v>
-      </c>
-      <c r="E8">
-        <v>40000</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>